<commit_message>
Added styling to Home page
</commit_message>
<xml_diff>
--- a/public/data/punjab.xlsx
+++ b/public/data/punjab.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\public_system_optimization\public\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CB91A37-E5D0-4A50-B355-8CD454E5DA6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B16AC596-F0E6-4383-9D0F-1C2F172F4B9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1860" yWindow="3585" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet7" sheetId="9" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Amritsar</t>
   </si>
@@ -108,14 +108,31 @@
   </si>
   <si>
     <t>Muktsar</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>supply</t>
+  </si>
+  <si>
+    <t>demand</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -143,11 +160,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -462,10 +480,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="A3" sqref="A3:C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -476,266 +494,277 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1">
-        <v>889874.4</v>
-      </c>
-      <c r="C1">
-        <v>891518.39999999979</v>
+      <c r="A1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="B2">
-        <v>197000</v>
+        <v>889874.4</v>
       </c>
       <c r="C2">
-        <v>169871.39999999994</v>
+        <v>891518.39999999979</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="B3">
-        <v>483840</v>
+        <v>197000</v>
       </c>
       <c r="C3">
-        <v>485399.40000000014</v>
+        <v>169871.39999999994</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="B4">
-        <v>304000</v>
+        <v>483840</v>
       </c>
       <c r="C4">
-        <v>211055.99999999991</v>
+        <v>485399.40000000014</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="B5">
-        <v>254900</v>
+        <v>304000</v>
       </c>
       <c r="C5">
-        <v>207442.19999999995</v>
+        <v>211055.99999999991</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="B6">
-        <v>667500</v>
+        <v>254900</v>
       </c>
       <c r="C6">
-        <v>488700.59999999974</v>
+        <v>207442.19999999995</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B7">
-        <v>792000</v>
+        <v>667500</v>
       </c>
       <c r="C7">
-        <v>347565.60000000027</v>
+        <v>488700.59999999974</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="B8">
-        <v>984500</v>
+        <v>792000</v>
       </c>
       <c r="C8">
-        <v>606942.00000000012</v>
+        <v>347565.60000000027</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B9">
-        <v>709700</v>
+        <v>984500</v>
       </c>
       <c r="C9">
-        <v>493399.20000000019</v>
+        <v>606942.00000000012</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B10">
-        <v>1337460</v>
+        <v>709700</v>
       </c>
       <c r="C10">
-        <v>651744.00000000105</v>
+        <v>493399.20000000019</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B11">
-        <v>273920</v>
+        <v>1337460</v>
       </c>
       <c r="C11">
-        <v>240044.99999999997</v>
+        <v>651744.00000000105</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="B12">
-        <v>513600</v>
+        <v>273920</v>
       </c>
       <c r="C12">
-        <v>531418.80000000016</v>
+        <v>240044.99999999997</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="B13">
-        <v>680200</v>
+        <v>513600</v>
       </c>
       <c r="C13">
-        <v>489763.19999999995</v>
+        <v>531418.80000000016</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B14">
-        <v>287000</v>
+        <v>680200</v>
       </c>
       <c r="C14">
-        <v>146045.39999999997</v>
+        <v>489763.19999999995</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="B15">
-        <v>1358550</v>
+        <v>287000</v>
       </c>
       <c r="C15">
-        <v>255261.20000000022</v>
+        <v>146045.39999999997</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B16">
-        <v>917520</v>
+        <v>1358550</v>
       </c>
       <c r="C16">
-        <v>315155.39999999991</v>
+        <v>255261.20000000022</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B17">
-        <v>735500</v>
+        <v>917520</v>
       </c>
       <c r="C17">
-        <v>364441.20000000013</v>
+        <v>315155.39999999991</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="B18">
-        <v>258000</v>
+        <v>735500</v>
       </c>
       <c r="C18">
-        <v>230483.99999999965</v>
+        <v>364441.20000000013</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="B19">
-        <v>947330</v>
+        <v>258000</v>
       </c>
       <c r="C19">
-        <v>594239.39999999956</v>
+        <v>230483.99999999965</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="B20">
-        <v>410800</v>
+        <v>947330</v>
       </c>
       <c r="C20">
-        <v>219812.40000000008</v>
+        <v>594239.39999999956</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B21">
-        <v>1127500</v>
+        <v>410800</v>
       </c>
       <c r="C21">
-        <v>430935.60000000056</v>
+        <v>219812.40000000008</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="B22">
-        <v>280800</v>
+        <v>1127500</v>
       </c>
       <c r="C22">
-        <v>261364.20000000022</v>
+        <v>430935.60000000056</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="B23">
-        <v>331500</v>
+        <v>280800</v>
       </c>
       <c r="C23">
-        <v>200716.80000000008</v>
+        <v>261364.20000000022</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B24">
+        <v>331500</v>
+      </c>
+      <c r="C24">
+        <v>200716.80000000008</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B24">
+      <c r="B25">
         <v>467000</v>
       </c>
-      <c r="C24">
+      <c r="C25">
         <v>466067.15000000008</v>
       </c>
     </row>

</xml_diff>